<commit_message>
add update tenant and profile url
</commit_message>
<xml_diff>
--- a/Tenant Test Plan.xlsx
+++ b/Tenant Test Plan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan_PC\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan_PC\Projects\RoomRv3-Backend\tenant-service\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{95965FBA-81E4-49FB-AC5E-D4CD7C8EEC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8EA21EF-FCCF-4B77-9A3F-C1DA3A4A86DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="23040" windowHeight="12204" xr2:uid="{910B9591-AAF6-41F1-BB09-D09732E5F0B0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>Test Name</t>
   </si>
@@ -885,6 +885,15 @@
   </si>
   <si>
     <t>HTTP 200</t>
+  </si>
+  <si>
+    <t>Tenant_Service_update_tenant_returns_successfully</t>
+  </si>
+  <si>
+    <t>Tenant_Service_rejects_invalid_state</t>
+  </si>
+  <si>
+    <t>HTTP 400</t>
   </si>
 </sst>
 </file>
@@ -1274,10 +1283,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{486F18B0-E8A3-4077-8B75-158E8CBC49E2}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:A22"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1442,6 +1451,22 @@
         <v>31</v>
       </c>
     </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>